<commit_message>
clean ui with hidden some id and class
</commit_message>
<xml_diff>
--- a/product/Kết quả quay số.xlsx
+++ b/product/Kết quả quay số.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -398,75 +398,69 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Giải đặc biệt</v>
+        <v>Giải</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Giải nhất</v>
+        <v>Giải</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" t="str">
-        <v xml:space="preserve">Kỹ thuật </v>
-      </c>
-      <c r="C5" t="str">
-        <v>GEM</v>
-      </c>
-      <c r="D5" t="str">
-        <v xml:space="preserve">Kỹ thuật </v>
+      <c r="A5" t="str">
+        <v>Giải</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" t="str">
-        <v>Kinh doanh</v>
-      </c>
-      <c r="C6" t="str">
-        <v>IN HOSPITALITY</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Kinh doanh</v>
+      <c r="A6" t="str">
+        <v>Giải</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" t="str">
-        <v>IN HOLD</v>
-      </c>
-      <c r="C7" t="str">
-        <v>IN HOLDINGS</v>
-      </c>
-      <c r="D7" t="str">
-        <v>IN HOLD</v>
+      <c r="A7" t="str">
+        <v>Giải</v>
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="str">
+        <v>White Palace</v>
+      </c>
       <c r="B8" t="str">
-        <v>Sản xuất</v>
+        <v>Bếp Convention</v>
       </c>
       <c r="C8" t="str">
-        <v>Meta Foods</v>
+        <v>Phạm Văn Đồng</v>
       </c>
       <c r="D8" t="str">
-        <v>Sản xuất</v>
+        <v>Bếp Convention White Palace Phạm Văn Đồng</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>IN META</v>
+        <v>White Palace</v>
       </c>
       <c r="B9" t="str">
-        <v>HCNS</v>
+        <v>Bảo vệ</v>
       </c>
       <c r="C9" t="str">
-        <v>CONVENTION</v>
+        <v>Võ Văn Kiệt</v>
       </c>
       <c r="D9" t="str">
-        <v>HCNS (IN+META+CONVENTION)</v>
+        <v>Bảo vệ White Palace Võ Văn Kiệt</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>Giải nhì</v>
+        <v>123 Lê Lợi</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Crystal Jade</v>
+      </c>
+      <c r="C10" t="str">
+        <v>CJ</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Crystal Jade 123 Lê Lợi</v>
       </c>
     </row>
     <row r="11">
@@ -481,61 +475,61 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="str">
-        <v>187 Hai Bà Trưng</v>
-      </c>
       <c r="B12" t="str">
-        <v>Tib</v>
+        <v>BOM Operation</v>
       </c>
       <c r="C12" t="str">
-        <v>IN Dining</v>
+        <v>BOM</v>
       </c>
       <c r="D12" t="str">
-        <v>Tib 187 Hai Bà Trưng</v>
+        <v>BOM Operation</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>40</v>
+        <v>06</v>
       </c>
       <c r="B13" t="str">
-        <v>Dynasty House</v>
+        <v>Marina</v>
       </c>
       <c r="C13" t="str">
-        <v>Phùng Khắc Khoan</v>
+        <v>Nguyễn Bỉnh Khiêm</v>
       </c>
       <c r="D13" t="str">
-        <v>Dynasty House 40 Phùng Khắc Khoan</v>
+        <v>Marina 06 Nguyễn Bỉnh Khiêm</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="str">
-        <v>40 Phùng Khắc Khoan</v>
-      </c>
       <c r="B14" t="str">
-        <v>Sushi Tei</v>
+        <v>F&amp;B - Lễ Tân</v>
       </c>
       <c r="C14" t="str">
-        <v>IN Dining</v>
+        <v>GEM</v>
       </c>
       <c r="D14" t="str">
-        <v>Sushi Tei 40 Phùng Khắc Khoan</v>
+        <v>F&amp;B - Lễ Tân GEM</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="str">
-        <v>The Log</v>
+        <v xml:space="preserve">Kỹ thuật </v>
       </c>
       <c r="C15" t="str">
+        <v>GEM</v>
+      </c>
+      <c r="D15" t="str">
+        <v>Kỹ thuật GEM</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="str">
+        <v>Bảo vệ</v>
+      </c>
+      <c r="C16" t="str">
         <v>IN Dining</v>
       </c>
-      <c r="D15" t="str">
-        <v>The Log</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>Giải ba</v>
+      <c r="D16" t="str">
+        <v>Bảo vệ</v>
       </c>
     </row>
     <row r="17">
@@ -550,529 +544,261 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="str">
-        <v>White Palace</v>
-      </c>
       <c r="B18" t="str">
-        <v>F&amp;B</v>
+        <v>Marketing</v>
       </c>
       <c r="C18" t="str">
-        <v>Võ Văn Kiệt</v>
+        <v>IN HOSPITALITY</v>
       </c>
       <c r="D18" t="str">
-        <v>F&amp;B</v>
+        <v>Marketing</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="str">
-        <v>03 Hạ Long</v>
-      </c>
       <c r="B19" t="str">
-        <v>Marina</v>
+        <v>Sản xuất</v>
       </c>
       <c r="C19" t="str">
-        <v>Vũng Tàu</v>
+        <v>Meta Foods</v>
       </c>
       <c r="D19" t="str">
-        <v>Marina 03 Hạ Long VT</v>
+        <v>Sản xuất</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>172</v>
+        <v>03 Hạ Long</v>
       </c>
       <c r="B20" t="str">
-        <v>Jumbo</v>
+        <v>Marina</v>
       </c>
       <c r="C20" t="str">
-        <v>Nguyễn Đình Chiểu</v>
+        <v>Vũng Tàu</v>
       </c>
       <c r="D20" t="str">
-        <v>Jumbo 172 Nguyễn Đình Chiểu</v>
+        <v>Marina 03 Hạ Long Vũng Tàu</v>
       </c>
     </row>
     <row r="21">
+      <c r="A21" t="str">
+        <v>IN - META</v>
+      </c>
       <c r="B21" t="str">
-        <v>Phòng Kế Toán</v>
+        <v>HCNS</v>
       </c>
       <c r="C21" t="str">
-        <v>IN Dining</v>
+        <v>CONVENTION</v>
       </c>
       <c r="D21" t="str">
-        <v>Phòng Kế toán IN Dining</v>
+        <v>HCNS (IN+META+CONVENTION)</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="str">
-        <v>238 Pasteur</v>
-      </c>
       <c r="B22" t="str">
-        <v>Âu Lạc</v>
+        <v xml:space="preserve">IN HOTEL </v>
       </c>
       <c r="C22" t="str">
-        <v>IN Dining</v>
+        <v xml:space="preserve">IN HOTEL </v>
       </c>
       <c r="D22" t="str">
-        <v>Âu Lạc 238 Pasteur</v>
+        <v xml:space="preserve">IN HOTEL </v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>White Palace</v>
+        <v>72 Nguyễn Thị</v>
       </c>
       <c r="B23" t="str">
-        <v>ST &amp; HK</v>
+        <v>Shri</v>
       </c>
       <c r="C23" t="str">
-        <v>Hoàng Văn Thụ</v>
+        <v>Minh Khai</v>
       </c>
       <c r="D23" t="str">
-        <v>Stewarding&amp;Housekeeping</v>
+        <v>Shri 72 Nguyễn Thị Minh Khai</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="str">
-        <v>WM</v>
+        <v>Sản xuất</v>
       </c>
       <c r="C24" t="str">
-        <v>WM</v>
+        <v>Meta Foods</v>
       </c>
       <c r="D24" t="str">
-        <v>WM</v>
+        <v>Sản xuất</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>06</v>
+        <v xml:space="preserve">05 </v>
       </c>
       <c r="B25" t="str">
-        <v>Marina</v>
+        <v>Sushi Tei</v>
       </c>
       <c r="C25" t="str">
-        <v>Nguyễn Bỉnh Khiêm</v>
+        <v>Lý Tự Trọng</v>
       </c>
       <c r="D25" t="str">
-        <v>Marina 06 Nguyễn Bỉnh Khiêm</v>
+        <v>Sushi Tei 05 Lý Tự Trọng</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="str">
-        <v>IN DEV</v>
+        <v>Sản xuất</v>
       </c>
       <c r="C26" t="str">
-        <v>IN DEVELOPMENT</v>
+        <v>Meta Foods</v>
       </c>
       <c r="D26" t="str">
-        <v>IN DEV</v>
+        <v>Sản xuất</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Giải khuyến khích</v>
+        <v xml:space="preserve">131 </v>
+      </c>
+      <c r="B27" t="str">
+        <v>Sushi Tei</v>
+      </c>
+      <c r="C27" t="str">
+        <v>Nguyễn Huệ</v>
+      </c>
+      <c r="D27" t="str">
+        <v>Sushi Tei 131 Nguyễn Huệ</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>06</v>
+        <v xml:space="preserve">10A </v>
       </c>
       <c r="B28" t="str">
-        <v>Jumbo</v>
+        <v>Sushi Tei</v>
       </c>
       <c r="C28" t="str">
         <v>Trần Hưng Đạo</v>
       </c>
       <c r="D28" t="str">
-        <v>Jumbo 06 Trần Hưng Đạo</v>
+        <v>Sushi Tei 10A Trần Hưng Đạo</v>
       </c>
     </row>
     <row r="29">
+      <c r="A29" t="str">
+        <v xml:space="preserve">200A </v>
+      </c>
       <c r="B29" t="str">
-        <v>Bảo vệ</v>
+        <v>Sushi Tei</v>
       </c>
       <c r="C29" t="str">
-        <v>IN Dining</v>
+        <v>Lý Tự Trọng</v>
       </c>
       <c r="D29" t="str">
-        <v>Bảo vệ</v>
+        <v>Sushi Tei 200A Lý Tự Trọng</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="str">
-        <v>141 Nguyễn Huệ</v>
-      </c>
       <c r="B30" t="str">
-        <v>Sushi Tei</v>
+        <v>IN HOLD</v>
       </c>
       <c r="C30" t="str">
-        <v>IN Dining</v>
+        <v>IN HOLDINGS</v>
       </c>
       <c r="D30" t="str">
-        <v>Sushi Tei 141 Nguyễn Huệ</v>
+        <v>IN HOLD</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="str">
-        <v>White Palace</v>
-      </c>
       <c r="B31" t="str">
-        <v>WP - HVT</v>
+        <v>BOM Operation</v>
       </c>
       <c r="C31" t="str">
-        <v>Hoàng Văn Thụ</v>
+        <v>BOM</v>
       </c>
       <c r="D31" t="str">
-        <v>WP - HVT</v>
+        <v>BOM Operation</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="str">
-        <v>40</v>
-      </c>
       <c r="B32" t="str">
-        <v>Dynasty House</v>
+        <v>Bếp Convention</v>
       </c>
       <c r="C32" t="str">
-        <v>Phùng Khắc Khoan</v>
+        <v>GEM</v>
       </c>
       <c r="D32" t="str">
-        <v>Dynasty House 40 Phùng Khắc Khoan</v>
+        <v>Bếp Convention GEM</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="str">
-        <v>IN HOS</v>
+        <v>WM</v>
       </c>
       <c r="C33" t="str">
-        <v>IN HOSPITALITY</v>
+        <v>WM</v>
       </c>
       <c r="D33" t="str">
-        <v>IN HOS</v>
+        <v>WM</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>Kỹ thuật+QC+Thu mua+HK</v>
+        <v>CLDV - CL - RR</v>
       </c>
       <c r="B34" t="str">
-        <v>Khối Back Office</v>
+        <v>Ban Kiểm Soát</v>
       </c>
       <c r="C34" t="str">
-        <v>Meta Foods</v>
+        <v>IN HOSPITALITY</v>
       </c>
       <c r="D34" t="str">
-        <v>Khối Back office (Kỹ thuật+QC+Thu mua+HK)</v>
+        <v>Ban Kiểm soát chất lượng dịch vụ &amp; Ban Kiểm soát chất lượng và Quản lý rủi ro</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>06</v>
+        <v>40</v>
       </c>
       <c r="B35" t="str">
-        <v>Marina</v>
+        <v>Dynasty House</v>
       </c>
       <c r="C35" t="str">
-        <v>Nguyễn Bỉnh Khiêm</v>
+        <v>Phùng Khắc Khoan</v>
       </c>
       <c r="D35" t="str">
-        <v>Marina 06 Nguyễn Bỉnh Khiêm</v>
+        <v>Dynasty House 40 Phùng Khắc Khoan</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>White Palace</v>
+        <v>KT - QC - TM - HK</v>
       </c>
       <c r="B36" t="str">
-        <v>Bảo vệ</v>
+        <v>Khối Back Office</v>
       </c>
       <c r="C36" t="str">
-        <v>Phạm Văn Đồng</v>
+        <v>Meta Foods</v>
       </c>
       <c r="D36" t="str">
-        <v>Bảo vệ</v>
+        <v>Khối Back office (Kỹ thuật+QC+Thu mua+HK)</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>1065 Trần Hưng Đạo</v>
+        <v>79</v>
       </c>
       <c r="B37" t="str">
-        <v>Spice World</v>
+        <v>Caparccio</v>
       </c>
       <c r="C37" t="str">
-        <v>IN Dining</v>
+        <v>Hai Bà Trưng</v>
       </c>
       <c r="D37" t="str">
-        <v>Spice World 1065 Trần Hưng Đạo</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="str">
-        <v>White Palace</v>
-      </c>
-      <c r="B38" t="str">
-        <v>Bếp Convention</v>
-      </c>
-      <c r="C38" t="str">
-        <v>Phạm Văn Đồng</v>
-      </c>
-      <c r="D38" t="str">
-        <v>Bếp Convention</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="str">
-        <v>131 Nguyễn Huệ</v>
-      </c>
-      <c r="B39" t="str">
-        <v>Sushi Tei</v>
-      </c>
-      <c r="C39" t="str">
-        <v>IN Dining</v>
-      </c>
-      <c r="D39" t="str">
-        <v>Sushi Tei 131 Nguyễn Huệ</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="str">
-        <v>02 - 06</v>
-      </c>
-      <c r="B40" t="str">
-        <v>Dynasty House</v>
-      </c>
-      <c r="C40" t="str">
-        <v>Đồng Khởi</v>
-      </c>
-      <c r="D40" t="str">
-        <v>Dynasty House 02 - 06 Đồng Khởi</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="str">
-        <v>02A - 04 A</v>
-      </c>
-      <c r="B41" t="str">
-        <v>Crystal Jade</v>
-      </c>
-      <c r="C41" t="str">
-        <v>Tôn Đức Thắng</v>
-      </c>
-      <c r="D41" t="str">
-        <v>Crystal Jade 02A - 04 A Tôn Đức Thắng</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="B42" t="str">
-        <v>Kinh doanh</v>
-      </c>
-      <c r="C42" t="str">
-        <v>IN HOSPITALITY</v>
-      </c>
-      <c r="D42" t="str">
-        <v>Kinh doanh</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" t="str">
-        <v>The Log</v>
-      </c>
-      <c r="C43" t="str">
-        <v>IN Dining</v>
-      </c>
-      <c r="D43" t="str">
-        <v>The Log</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="str">
-        <v>120 Lý Thái Tổ</v>
-      </c>
-      <c r="B44" t="str">
-        <v>Sushi Tei</v>
-      </c>
-      <c r="C44" t="str">
-        <v>IN Dining</v>
-      </c>
-      <c r="D44" t="str">
-        <v>Sushi Tei 120 Lý Thái Tổ</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="str">
-        <v>White Palace</v>
-      </c>
-      <c r="B45" t="str">
-        <v>F&amp;B</v>
-      </c>
-      <c r="C45" t="str">
-        <v>Phạm Văn Đồng</v>
-      </c>
-      <c r="D45" t="str">
-        <v>F&amp;B</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="str">
-        <v>123 Lê Lợi</v>
-      </c>
-      <c r="B46" t="str">
-        <v>Crystal Jade</v>
-      </c>
-      <c r="C46" t="str">
-        <v>CJ</v>
-      </c>
-      <c r="D46" t="str">
-        <v>Crystal Jade 123 Lê Lợi</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47" t="str">
-        <v>GEM Cafe</v>
-      </c>
-      <c r="C47" t="str">
-        <v>IN Dining</v>
-      </c>
-      <c r="D47" t="str">
-        <v>GEM Cafe</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="str">
-        <v>CLDV+CL+RR</v>
-      </c>
-      <c r="B48" t="str">
-        <v>Ban Kiểm Soát</v>
-      </c>
-      <c r="C48" t="str">
-        <v>IN HOSPITALITY</v>
-      </c>
-      <c r="D48" t="str">
-        <v>Ban Kiểm soát chất lượng dịch vụ &amp; Ban Kiểm soát chất lượng và Quản lý rủi ro</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="str">
-        <v>120 Lý Thái Tổ</v>
-      </c>
-      <c r="B49" t="str">
-        <v>Spice World</v>
-      </c>
-      <c r="C49" t="str">
-        <v>IN Dining</v>
-      </c>
-      <c r="D49" t="str">
-        <v>Spice World 120 Lý Thái Tổ</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="str">
-        <v>72 Nguyễn Thị Minh Khai</v>
-      </c>
-      <c r="B50" t="str">
-        <v>Shri</v>
-      </c>
-      <c r="C50" t="str">
-        <v>IN Dining</v>
-      </c>
-      <c r="D50" t="str">
-        <v>Shri 72 Nguyễn Thị Minh Khai</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="str">
-        <v>02 - 06</v>
-      </c>
-      <c r="B51" t="str">
-        <v>Jumbo</v>
-      </c>
-      <c r="C51" t="str">
-        <v>Đồng Khởi</v>
-      </c>
-      <c r="D51" t="str">
-        <v>Jumbo 02 - 06 Đồng Khởi</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="B52" t="str">
-        <v>Hậu Cần</v>
-      </c>
-      <c r="C52" t="str">
-        <v>IN HOSPITALITY</v>
-      </c>
-      <c r="D52" t="str">
-        <v>Hậu Cần</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="str">
-        <v>White Palace</v>
-      </c>
-      <c r="B53" t="str">
-        <v>Giặt ủi</v>
-      </c>
-      <c r="C53" t="str">
-        <v>Phạm Văn Đồng</v>
-      </c>
-      <c r="D53" t="str">
-        <v>Giặt ủi</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="str">
-        <v>White Palace</v>
-      </c>
-      <c r="B54" t="str">
-        <v>Bảo vệ</v>
-      </c>
-      <c r="C54" t="str">
-        <v>Võ Văn Kiệt</v>
-      </c>
-      <c r="D54" t="str">
-        <v>Bảo vệ</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="B55" t="str">
-        <v>Phòng Bảo trì</v>
-      </c>
-      <c r="C55" t="str">
-        <v>IN Dining</v>
-      </c>
-      <c r="D55" t="str">
-        <v>Phòng Bảo trì</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="str">
-        <v>79</v>
-      </c>
-      <c r="B56" t="str">
-        <v>Caparccio</v>
-      </c>
-      <c r="C56" t="str">
-        <v>Hai Bà Trưng</v>
-      </c>
-      <c r="D56" t="str">
         <v>Caparccio 79 Hai Bà Trưng</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="str">
-        <v>40</v>
-      </c>
-      <c r="B57" t="str">
-        <v>Âu Lạc</v>
-      </c>
-      <c r="C57" t="str">
-        <v>Phùng Khắc Khoan</v>
-      </c>
-      <c r="D57" t="str">
-        <v>Âu Lạc 40 Phùng Khắc Khoan</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D57"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D37"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>